<commit_message>
Decreased number of experiments
</commit_message>
<xml_diff>
--- a/Data/Sensitivity Analysis Setup.xlsx
+++ b/Data/Sensitivity Analysis Setup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Dropbox\EPA\Q5\Agent Based Modelling\ABM-waste-recycling-in-NL\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{385A2A62-4DC4-420A-B35D-CF979516B3CE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A0245D19-FFBD-4412-A241-B7BE308B8E21}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14610" windowHeight="6150" xr2:uid="{82D752E7-81BE-4644-B888-D4D34F0F87C7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
   <si>
     <t>Variable</t>
   </si>
@@ -126,27 +126,12 @@
     <t>["recycling-target-increase" 15 16.5]</t>
   </si>
   <si>
-    <t>["month-before-target-increase" 120 132]</t>
-  </si>
-  <si>
     <t>["num-municipalities" 10 11]</t>
   </si>
   <si>
     <t>["num-RC" 5 6]</t>
   </si>
   <si>
-    <t>["month-before-technology-increase" 12 13]</t>
-  </si>
-  <si>
-    <t>["base-value-beta1" 0.4 0.44]</t>
-  </si>
-  <si>
-    <t>["base-value-beta2" 0.55 0.605]</t>
-  </si>
-  <si>
-    <t>["base-value-target-investment-tendency" 0.25 0.275]</t>
-  </si>
-  <si>
     <t>["recycling-target" 0.65 0.585]</t>
   </si>
   <si>
@@ -177,27 +162,12 @@
     <t>["recycling-target-increase" 15 13.5]</t>
   </si>
   <si>
-    <t>["month-before-target-increase" 120 108]</t>
-  </si>
-  <si>
-    <t>["base-value-beta1" 0.4 0.36]</t>
-  </si>
-  <si>
-    <t>["base-value-beta2" 0.55 0.495]</t>
-  </si>
-  <si>
-    <t>["base-value-target-investment-tendency" 0.25 0.225]</t>
-  </si>
-  <si>
     <t>["num-municipalities" 10 9]</t>
   </si>
   <si>
     <t>["num-RC" 5 4]</t>
   </si>
   <si>
-    <t>["month-before-technology-increase" 12 11]</t>
-  </si>
-  <si>
     <t>["recycling-target" 0.65 0.8125]</t>
   </si>
   <si>
@@ -228,27 +198,12 @@
     <t>["recycling-target-increase" 15 18.75]</t>
   </si>
   <si>
-    <t>["month-before-target-increase" 120 150]</t>
-  </si>
-  <si>
-    <t>["base-value-beta1" 0.4 0.5]</t>
-  </si>
-  <si>
-    <t>["base-value-beta2" 0.55 0.6875]</t>
-  </si>
-  <si>
-    <t>["base-value-target-investment-tendency" 0.25 0.3125]</t>
-  </si>
-  <si>
     <t>["num-municipalities" 10 13]</t>
   </si>
   <si>
     <t>["num-RC" 5 7]</t>
   </si>
   <si>
-    <t>["month-before-technology-increase" 12 15]</t>
-  </si>
-  <si>
     <t>["recycling-target" 0.65 0.4875]</t>
   </si>
   <si>
@@ -279,27 +234,12 @@
     <t>["recycling-target-increase" 15 11.25]</t>
   </si>
   <si>
-    <t>["month-before-target-increase" 120 90]</t>
-  </si>
-  <si>
-    <t>["base-value-beta1" 0.4 0.3]</t>
-  </si>
-  <si>
-    <t>["base-value-beta2" 0.55 0.4125]</t>
-  </si>
-  <si>
-    <t>["base-value-target-investment-tendency" 0.25 0.1875]</t>
-  </si>
-  <si>
     <t>["num-municipalities" 10 8]</t>
   </si>
   <si>
     <t>["num-RC" 5 3]</t>
   </si>
   <si>
-    <t>["month-before-technology-increase" 12 9]</t>
-  </si>
-  <si>
     <t>Sensitivity Analysis base run</t>
   </si>
   <si>
@@ -333,25 +273,10 @@
     <t>["recycling-target-increase" 15]</t>
   </si>
   <si>
-    <t>["month-before-target-increase" 120]</t>
-  </si>
-  <si>
-    <t>["base-value-beta1" 0.4]</t>
-  </si>
-  <si>
-    <t>["base-value-beta2" 0.55]</t>
-  </si>
-  <si>
-    <t>["base-value-target-investment-tendency" 0.25]</t>
-  </si>
-  <si>
     <t>["num-municipalities" 10]</t>
   </si>
   <si>
     <t>["num-RC" 5]</t>
-  </si>
-  <si>
-    <t>["month-before-technology-increase" 12]</t>
   </si>
 </sst>
 </file>
@@ -763,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA930786-EA83-4091-990D-DF3CEF94400D}">
-  <dimension ref="A1:I75"/>
+  <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:A37"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I44" sqref="I44:I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,7 +1021,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1119,11 +1044,11 @@
         <f t="shared" si="3"/>
         <v>0.30000000000000004</v>
       </c>
-      <c r="I13" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I13" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1146,9 +1071,7 @@
         <f t="shared" si="3"/>
         <v>0.41250000000000003</v>
       </c>
-      <c r="I14" s="5" t="s">
-        <v>38</v>
-      </c>
+      <c r="I14" s="8"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1173,8 +1096,8 @@
         <f t="shared" si="3"/>
         <v>0.1875</v>
       </c>
-      <c r="I15" s="5" t="s">
-        <v>39</v>
+      <c r="I15" s="4" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1202,7 +1125,7 @@
       </c>
       <c r="H16" s="9"/>
       <c r="I16" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1230,10 +1153,10 @@
       </c>
       <c r="H17" s="9"/>
       <c r="I17" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
@@ -1257,26 +1180,28 @@
         <v>9</v>
       </c>
       <c r="H18" s="9"/>
-      <c r="I18" s="6" t="s">
-        <v>36</v>
+      <c r="I18" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:9" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
+      <c r="I19" s="5" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="20" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="H20" s="8"/>
-      <c r="I20" s="4" t="s">
-        <v>21</v>
+      <c r="I20" s="5" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="H21" s="8"/>
       <c r="I21" s="5" t="s">
@@ -1285,7 +1210,7 @@
     </row>
     <row r="22" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="H22" s="8"/>
       <c r="I22" s="5" t="s">
@@ -1294,7 +1219,7 @@
     </row>
     <row r="23" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="H23" s="8"/>
       <c r="I23" s="5" t="s">
@@ -1303,7 +1228,7 @@
     </row>
     <row r="24" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="H24" s="8"/>
       <c r="I24" s="5" t="s">
@@ -1312,7 +1237,7 @@
     </row>
     <row r="25" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="H25" s="8"/>
       <c r="I25" s="5" t="s">
@@ -1321,323 +1246,212 @@
     </row>
     <row r="26" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="H26" s="8"/>
       <c r="I26" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="H27" s="8"/>
-      <c r="I27" s="5" t="s">
+      <c r="I27" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="H28" s="8"/>
-      <c r="I28" s="5" t="s">
-        <v>47</v>
-      </c>
+      <c r="I28" s="8"/>
     </row>
     <row r="29" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="H29" s="8"/>
-      <c r="I29" s="5" t="s">
-        <v>48</v>
+      <c r="I29" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="30" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="H30" s="8"/>
       <c r="I30" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="H31" s="8"/>
       <c r="I31" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
-        <v>103</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="6" t="s">
+        <v>83</v>
       </c>
       <c r="H32" s="8"/>
       <c r="I32" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
-        <v>104</v>
-      </c>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="33" spans="8:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H33" s="8"/>
       <c r="I33" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
-        <v>105</v>
-      </c>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="8:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H34" s="8"/>
       <c r="I34" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
-        <v>106</v>
-      </c>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="8:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H35" s="8"/>
       <c r="I35" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
-        <v>107</v>
-      </c>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="8:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H36" s="8"/>
       <c r="I36" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="8:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H37" s="8"/>
+      <c r="I37" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="8:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H38" s="8"/>
+      <c r="I38" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="1:9" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="H37" s="8"/>
-      <c r="I37" s="6" t="s">
+    <row r="39" spans="8:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H39" s="8"/>
+      <c r="I39" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="1:9" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
-    </row>
-    <row r="39" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H39" s="8"/>
-      <c r="I39" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="8:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H40" s="8"/>
       <c r="I40" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="41" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="8:9" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H41" s="8"/>
-      <c r="I41" s="5" t="s">
+      <c r="I41" s="6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="42" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="8:9" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H42" s="8"/>
-      <c r="I42" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I42" s="8"/>
+    </row>
+    <row r="43" spans="8:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H43" s="8"/>
-      <c r="I43" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I43" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" spans="8:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H44" s="8"/>
       <c r="I44" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="8:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H45" s="8"/>
       <c r="I45" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" spans="8:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H46" s="8"/>
       <c r="I46" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="47" spans="8:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H47" s="8"/>
       <c r="I47" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="48" spans="8:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H48" s="8"/>
       <c r="I48" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="49" spans="8:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H49" s="8"/>
       <c r="I49" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="50" spans="8:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H50" s="8"/>
       <c r="I50" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="51" spans="8:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H51" s="8"/>
       <c r="I51" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="52" spans="8:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H52" s="8"/>
       <c r="I52" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="53" spans="8:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H53" s="8"/>
       <c r="I53" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="54" spans="8:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H54" s="8"/>
       <c r="I54" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="55" spans="8:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="55" spans="8:9" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H55" s="8"/>
-      <c r="I55" s="5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="56" spans="8:9" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I55" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="56" spans="8:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H56" s="8"/>
-      <c r="I56" s="6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="57" spans="8:9" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I56"/>
+    </row>
+    <row r="57" spans="8:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H57" s="8"/>
-      <c r="I57" s="8"/>
+      <c r="I57"/>
     </row>
     <row r="58" spans="8:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H58" s="8"/>
-      <c r="I58" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="59" spans="8:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H59" s="8"/>
-      <c r="I59" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="60" spans="8:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H60" s="8"/>
-      <c r="I60" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="61" spans="8:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H61" s="8"/>
-      <c r="I61" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="62" spans="8:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H62" s="8"/>
-      <c r="I62" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="63" spans="8:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H63" s="8"/>
-      <c r="I63" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="64" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="I64" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="65" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I65" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="66" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I66" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="67" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I67" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="68" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I68" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="69" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I69" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="70" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I70" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="71" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I71" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="72" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I72" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="73" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I73" s="5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="74" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I74" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="75" spans="9:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I75" s="6" t="s">
-        <v>90</v>
-      </c>
+      <c r="I58"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>